<commit_message>
20250411 LC3WP + LC1EP
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202504/EuTaxonomyPocket_after_Committee.xlsx
+++ b/GUI + Reviews/202504/EuTaxonomyPocket_after_Committee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-IndexTeam\3. Committees\I. LC100\2025_03 ANNUAL REVIEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202504/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7780B5C7-4E39-43A1-9645-AF0B51882C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{7780B5C7-4E39-43A1-9645-AF0B51882C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF8EBC7-4DFE-41F4-B4BA-F8CD6B996650}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" activeTab="2" xr2:uid="{8CAAB48C-2B86-471E-AE3A-557AA03E146E}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{8CAAB48C-2B86-471E-AE3A-557AA03E146E}"/>
   </bookViews>
   <sheets>
     <sheet name="Europe" sheetId="1" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>INPOST</t>
   </si>
   <si>
-    <t>DK0010219153</t>
-  </si>
-  <si>
     <t>WK2NJZ-R</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>EDP RENOVAVEIS</t>
+  </si>
+  <si>
+    <t>DK0063855168</t>
   </si>
 </sst>
 </file>
@@ -602,19 +602,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0A0883-6B87-41A5-A159-714D3DA2F9C3}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -656,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -670,7 +670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -684,7 +684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -698,7 +698,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -712,7 +712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -726,7 +726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -740,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -754,7 +754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -768,7 +768,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -782,7 +782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -796,7 +796,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -810,18 +810,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -840,15 +840,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -876,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -890,21 +890,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -918,7 +918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -932,7 +932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -946,7 +946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -960,7 +960,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -974,35 +974,35 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
         <v>50</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1030,18 +1030,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1056,19 +1056,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F140CC-06C5-42D2-A2D8-9A27B336C18D}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E2:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.3046875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1264,18 +1264,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>